<commit_message>
added function to parse charging mechanism text into dict
</commit_message>
<xml_diff>
--- a/OCS/OCS_1.xlsx
+++ b/OCS/OCS_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joachim.Wan\Desktop\OpsProject\dccs_generator\OCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CA173F-3A0C-4D1C-8D84-B35172C9B1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6EF2AF-342F-4361-8910-A871D0914C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCS Input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Contract Title:</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Cost Bucket</t>
-  </si>
-  <si>
     <t>Description 1</t>
   </si>
   <si>
@@ -138,6 +135,24 @@
   </si>
   <si>
     <t>C.MY.F14.DD.22.001.1094D</t>
+  </si>
+  <si>
+    <t>Charging Mechanism</t>
+  </si>
+  <si>
+    <t>1 unit/day recur daily from start date 01/01/2023 to end phase 50</t>
+  </si>
+  <si>
+    <t>1  unit/day recur weekly on Monday Wednesday from start date 01/01/2023 to end date 01/01/2024</t>
+  </si>
+  <si>
+    <t>1.2 unit/day no recurrence from start date 01/03/2023</t>
+  </si>
+  <si>
+    <t>0.5 unit/day no recurrence from end phase 15</t>
+  </si>
+  <si>
+    <t>Cost Group</t>
   </si>
 </sst>
 </file>
@@ -173,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -251,11 +266,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -264,13 +290,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+  <dxfs count="16">
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -301,6 +327,23 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -498,22 +541,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8352A9AC-9193-473D-976F-D2AC42C7E8B8}" name="OCSTable" displayName="OCSTable" ref="A10:K14" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A10:K14" xr:uid="{8352A9AC-9193-473D-976F-D2AC42C7E8B8}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{0150FA52-A459-4732-9611-5BE4BABC6A72}" name="Item Number" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{B24C48AE-5AA5-4AE9-A360-1BD09733FF90}" name="Description" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{E84A40EB-8DDC-466C-A824-DE1DA46B72D6}" name="SAP Element Number" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{565BADD0-BF7C-43D2-9F41-459A98917CB5}" name="Quantity" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{6090D70F-3B5B-4952-928D-678757DE5FA5}" name="Unit of Measure" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4B681FFC-AC05-4352-B797-FBE6682057EA}" name="Estimated Duration" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{9AAB615E-A271-44BA-B009-A6CF615CF1CA}" name="Currency" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{F0E88AAC-7899-4177-B17A-B75E95D77B3A}" name="SAP Unit Price" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{2EED73C0-3A8D-4536-80BC-5D3B70D3F754}" name="Total Price" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8352A9AC-9193-473D-976F-D2AC42C7E8B8}" name="OCSTable" displayName="OCSTable" ref="A10:L14" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A10:L14" xr:uid="{8352A9AC-9193-473D-976F-D2AC42C7E8B8}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{0150FA52-A459-4732-9611-5BE4BABC6A72}" name="Item Number" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{B24C48AE-5AA5-4AE9-A360-1BD09733FF90}" name="Description" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{E84A40EB-8DDC-466C-A824-DE1DA46B72D6}" name="SAP Element Number" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{565BADD0-BF7C-43D2-9F41-459A98917CB5}" name="Quantity" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{6090D70F-3B5B-4952-928D-678757DE5FA5}" name="Unit of Measure" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{4B681FFC-AC05-4352-B797-FBE6682057EA}" name="Estimated Duration" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{9AAB615E-A271-44BA-B009-A6CF615CF1CA}" name="Currency" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{F0E88AAC-7899-4177-B17A-B75E95D77B3A}" name="SAP Unit Price" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{2EED73C0-3A8D-4536-80BC-5D3B70D3F754}" name="Total Price" dataDxfId="3">
       <calculatedColumnFormula>OCSTable[[#This Row],[Quantity]]*OCSTable[[#This Row],[Estimated Duration]]*OCSTable[[#This Row],[SAP Unit Price]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{9ACA5C19-B726-493A-BC5C-5AAA531BC2EF}" name="Remarks" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{67229ADC-C2E1-45EC-A52C-05472616ACAE}" name="Cost Bucket" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{67229ADC-C2E1-45EC-A52C-05472616ACAE}" name="Cost Group" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{EB19B413-E4B3-4048-B576-D2C3116BD861}" name="Charging Mechanism" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -782,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +837,7 @@
     <col min="1" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -803,43 +847,43 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -849,7 +893,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -859,7 +903,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -891,30 +935,33 @@
         <v>19</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="6">
         <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="6">
         <v>1000</v>
@@ -927,28 +974,31 @@
       <c r="K11" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>2</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="6">
         <v>2</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="6">
         <v>20</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="6">
         <v>1500</v>
@@ -961,28 +1011,31 @@
       <c r="K12" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="6">
         <v>3</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="6">
         <v>30</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="6">
         <v>5000</v>
@@ -995,28 +1048,31 @@
       <c r="K13" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="6">
         <v>4</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="6">
         <v>40</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" s="6">
         <v>10000</v>
@@ -1028,6 +1084,9 @@
       <c r="J14" s="6"/>
       <c r="K14" s="7">
         <v>20</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated date well table to assist withtariff charging
</commit_message>
<xml_diff>
--- a/OCS/OCS_1.xlsx
+++ b/OCS/OCS_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joachim.Wan\Desktop\OpsProject\dccs_generator\OCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6EF2AF-342F-4361-8910-A871D0914C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2C828E-378E-438D-AFBD-72CBBDFD7308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15720" yWindow="7485" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCS Input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Contract Title:</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Cost Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -826,11 +829,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1087,6 +1088,11 @@
       </c>
       <c r="L14" s="8" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added charging mechanism based on parsed information
</commit_message>
<xml_diff>
--- a/OCS/OCS_1.xlsx
+++ b/OCS/OCS_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joachim.Wan\Desktop\OpsProject\dccs_generator\OCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2C828E-378E-438D-AFBD-72CBBDFD7308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719214A5-4970-42C9-B535-BE2B40F61C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15720" yWindow="7485" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCS Input" sheetId="1" r:id="rId1"/>
@@ -140,22 +140,22 @@
     <t>Charging Mechanism</t>
   </si>
   <si>
-    <t>1 unit/day recur daily from start date 01/01/2023 to end phase 50</t>
-  </si>
-  <si>
-    <t>1  unit/day recur weekly on Monday Wednesday from start date 01/01/2023 to end date 01/01/2024</t>
-  </si>
-  <si>
-    <t>1.2 unit/day no recurrence from start date 01/03/2023</t>
-  </si>
-  <si>
-    <t>0.5 unit/day no recurrence from end phase 15</t>
-  </si>
-  <si>
     <t>Cost Group</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>1 unit/day from start phase 50 to end phase 50 for maximum 7 occurrences</t>
+  </si>
+  <si>
+    <t>1.3 unit/day from 2023/04/01 to end phase 50</t>
+  </si>
+  <si>
+    <t>1.4 unit/day from 2023/04/01 to 2023/05/02 for maximum 7 occurrences</t>
+  </si>
+  <si>
+    <t>2.1 unit/day for {'GK-P527B': [5,10,15,20], 'GK-W526C':[5]} for maximum 15 occurrences</t>
   </si>
 </sst>
 </file>
@@ -831,7 +831,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -936,7 +938,7 @@
         <v>19</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>33</v>
@@ -976,7 +978,7 @@
         <v>15</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1013,7 +1015,7 @@
         <v>15</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1050,7 +1052,7 @@
         <v>15</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1087,12 +1089,12 @@
         <v>20</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>